<commit_message>
fixed some bugs for the hours and aligning
</commit_message>
<xml_diff>
--- a/2522_monthly_analysis.xlsx
+++ b/2522_monthly_analysis.xlsx
@@ -60052,88 +60052,110 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>8</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>08:00 AM</t>
+        </is>
       </c>
       <c r="B2" t="n">
         <v>52</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>9</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>09:00 AM</t>
+        </is>
       </c>
       <c r="B3" t="n">
         <v>64</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>10</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>10:00 AM</t>
+        </is>
       </c>
       <c r="B4" t="n">
         <v>68</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>11</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>11:00 AM</t>
+        </is>
       </c>
       <c r="B5" t="n">
         <v>19</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>12</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>12:00 PM</t>
+        </is>
       </c>
       <c r="B6" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>13</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>01:00 PM</t>
+        </is>
       </c>
       <c r="B7" t="n">
         <v>53</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>14</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>02:00 PM</t>
+        </is>
       </c>
       <c r="B8" t="n">
         <v>50</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>15</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>03:00 PM</t>
+        </is>
       </c>
       <c r="B9" t="n">
         <v>41</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>16</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>04:00 PM</t>
+        </is>
       </c>
       <c r="B10" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>17</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>05:00 PM</t>
+        </is>
       </c>
       <c r="B11" t="n">
         <v>27</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>18</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>06:00 PM</t>
+        </is>
       </c>
       <c r="B12" t="n">
         <v>2</v>

</xml_diff>